<commit_message>
code fiddling for nicer figures
</commit_message>
<xml_diff>
--- a/Data/LMMRefs_adaptabilitytoGMM.xlsx
+++ b/Data/LMMRefs_adaptabilitytoGMM.xlsx
@@ -926,15 +926,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="69.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.5546875" customWidth="1"/>
   </cols>
@@ -1141,6 +1141,9 @@
       <c r="G11" s="3" t="s">
         <v>134</v>
       </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
@@ -1164,6 +1167,9 @@
       <c r="H12" s="3" t="s">
         <v>138</v>
       </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
@@ -1190,6 +1196,9 @@
       <c r="I13" s="3" t="s">
         <v>138</v>
       </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
@@ -1215,6 +1224,9 @@
       </c>
       <c r="J14" t="s">
         <v>138</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>